<commit_message>
some edits based on MG
</commit_message>
<xml_diff>
--- a/results/candidate_contamination.xlsx
+++ b/results/candidate_contamination.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jincheng/Projects/seeding-study/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FEF83ED-B048-FB47-B009-DD26229B8E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401C61B1-AACD-444E-9E81-613F7431EC18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="460" windowWidth="25040" windowHeight="28340"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="25040" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="candidate_contamination" sheetId="1" r:id="rId1"/>
@@ -285,12 +285,6 @@
     <t>veronii</t>
   </si>
   <si>
-    <t>Mean relative abundance</t>
-  </si>
-  <si>
-    <t>Median relative abundance</t>
-  </si>
-  <si>
     <t>Prevalence</t>
   </si>
   <si>
@@ -301,12 +295,18 @@
   </si>
   <si>
     <t>Fecal samples</t>
+  </si>
+  <si>
+    <t>Mean Count</t>
+  </si>
+  <si>
+    <t>Median Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -639,7 +639,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -755,42 +755,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dashed">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="dashed">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="dashed">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right style="dashed">
-        <color indexed="64"/>
-      </right>
-      <top style="dashed">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right style="dashed">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="dashed">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -841,29 +815,24 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1219,7 +1188,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1229,86 +1198,94 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="16" width="11.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="J2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:17" ht="27" x14ac:dyDescent="0.2">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="K2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>85</v>
+      <c r="O2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="Q2" t="s">
         <v>0</v>
@@ -1318,43 +1295,43 @@
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="8">
+      <c r="G3" s="5"/>
+      <c r="H3" s="6">
         <v>0.20370370370370369</v>
       </c>
-      <c r="I3" s="8">
-        <v>1.5384527461432099E-2</v>
-      </c>
-      <c r="J3" s="8">
-        <v>7.9096045197740092E-3</v>
-      </c>
-      <c r="K3" s="8">
+      <c r="I3" s="7">
+        <v>31.939393939393899</v>
+      </c>
+      <c r="J3" s="7">
+        <v>13</v>
+      </c>
+      <c r="K3" s="6">
         <v>0.73681318681318686</v>
       </c>
-      <c r="L3" s="8">
-        <v>1.15230852471911E-2</v>
-      </c>
-      <c r="M3" s="8">
-        <v>1.5649006999374001E-3</v>
-      </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
+      <c r="L3" s="7">
+        <v>504.31096196867998</v>
+      </c>
+      <c r="M3" s="7">
+        <v>36</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
       <c r="Q3" t="s">
         <v>20</v>
       </c>
@@ -1363,42 +1340,42 @@
       <c r="A4" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="8">
+      <c r="G4" s="5"/>
+      <c r="H4" s="6">
         <v>0.23456790123456789</v>
       </c>
-      <c r="I4" s="8">
-        <v>0.19462606613381001</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.19496082798394901</v>
-      </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="8">
+      <c r="I4" s="7">
+        <v>2060.5</v>
+      </c>
+      <c r="J4" s="7">
+        <v>25.5</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="6">
         <v>0.82314881380301941</v>
       </c>
-      <c r="O4" s="8">
-        <v>0.14218257414254301</v>
-      </c>
-      <c r="P4" s="8">
-        <v>4.48258359241165E-2</v>
+      <c r="O4" s="7">
+        <v>7338.1912663755502</v>
+      </c>
+      <c r="P4" s="7">
+        <v>1058</v>
       </c>
       <c r="Q4" t="s">
         <v>40</v>
@@ -1408,44 +1385,44 @@
       <c r="A5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="6">
         <v>0.11728395061728394</v>
       </c>
-      <c r="I5" s="8">
-        <v>4.3070700099462497E-2</v>
-      </c>
-      <c r="J5" s="8">
-        <v>2.75665399239544E-2</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="8">
+      <c r="I5" s="7">
+        <v>1225.0606060606101</v>
+      </c>
+      <c r="J5" s="7">
+        <v>19</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="6">
         <v>0.3666427030913012</v>
       </c>
-      <c r="O5" s="8">
-        <v>3.4607603603476401E-2</v>
-      </c>
-      <c r="P5" s="8">
-        <v>3.0135701780592602E-3</v>
+      <c r="O5" s="7">
+        <v>9170.5032467532492</v>
+      </c>
+      <c r="P5" s="7">
+        <v>232.5</v>
       </c>
       <c r="Q5" t="s">
         <v>34</v>
@@ -1455,42 +1432,42 @@
       <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="8">
+      <c r="G6" s="5"/>
+      <c r="H6" s="6">
         <v>0.20370370370370369</v>
       </c>
-      <c r="I6" s="8">
-        <v>0.14098156339763401</v>
-      </c>
-      <c r="J6" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="8">
+      <c r="I6" s="7">
+        <v>424.947368421053</v>
+      </c>
+      <c r="J6" s="7">
+        <v>25</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="6">
         <v>0.66427030913012219</v>
       </c>
-      <c r="O6" s="8">
-        <v>0.124696674673757</v>
-      </c>
-      <c r="P6" s="8">
-        <v>1.25219984429253E-2</v>
+      <c r="O6" s="7">
+        <v>2159.9607843137301</v>
+      </c>
+      <c r="P6" s="7">
+        <v>75</v>
       </c>
       <c r="Q6" t="s">
         <v>38</v>
@@ -1500,43 +1477,43 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="8">
+      <c r="G7" s="5"/>
+      <c r="H7" s="6">
         <v>0.1419753086419753</v>
       </c>
-      <c r="I7" s="8">
-        <v>4.0870685821972702E-2</v>
-      </c>
-      <c r="J7" s="8">
-        <v>1.20481927710843E-2</v>
-      </c>
-      <c r="K7" s="8">
+      <c r="I7" s="7">
+        <v>251.77966101694901</v>
+      </c>
+      <c r="J7" s="7">
+        <v>41</v>
+      </c>
+      <c r="K7" s="6">
         <v>0.1357142857142857</v>
       </c>
-      <c r="L7" s="8">
-        <v>5.9137462659229201E-3</v>
-      </c>
-      <c r="M7" s="8">
-        <v>1.8992403038784499E-3</v>
-      </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
+      <c r="L7" s="7">
+        <v>3810.9793814433001</v>
+      </c>
+      <c r="M7" s="7">
+        <v>440.5</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
       <c r="Q7" t="s">
         <v>10</v>
       </c>
@@ -1545,43 +1522,43 @@
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="8">
+      <c r="G8" s="5"/>
+      <c r="H8" s="6">
         <v>0.26543209876543211</v>
       </c>
-      <c r="I8" s="8">
-        <v>7.3674374248827695E-2</v>
-      </c>
-      <c r="J8" s="8">
-        <v>6.41891891891892E-2</v>
-      </c>
-      <c r="K8" s="8">
+      <c r="I8" s="7">
+        <v>16.2173913043478</v>
+      </c>
+      <c r="J8" s="7">
+        <v>10</v>
+      </c>
+      <c r="K8" s="6">
         <v>0.33736263736263739</v>
       </c>
-      <c r="L8" s="8">
-        <v>1.3127057129158799E-2</v>
-      </c>
-      <c r="M8" s="8">
-        <v>4.4230792114687998E-3</v>
-      </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
+      <c r="L8" s="7">
+        <v>46.8704453441296</v>
+      </c>
+      <c r="M8" s="7">
+        <v>25</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
       <c r="Q8" t="s">
         <v>26</v>
       </c>
@@ -1590,41 +1567,41 @@
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="8">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6">
         <v>0.18518518518518517</v>
       </c>
-      <c r="I9" s="8">
-        <v>4.3230610909175099E-2</v>
-      </c>
-      <c r="J9" s="8">
-        <v>1.93768228941061E-2</v>
-      </c>
-      <c r="K9" s="8">
+      <c r="I9" s="7">
+        <v>43.093023255814003</v>
+      </c>
+      <c r="J9" s="7">
+        <v>28</v>
+      </c>
+      <c r="K9" s="6">
         <v>0.86208791208791213</v>
       </c>
-      <c r="L9" s="8">
-        <v>4.8742134917398303E-2</v>
-      </c>
-      <c r="M9" s="8">
-        <v>2.2419102155475101E-2</v>
-      </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
+      <c r="L9" s="7">
+        <v>153.71172638436499</v>
+      </c>
+      <c r="M9" s="7">
+        <v>67.5</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
       <c r="Q9" t="s">
         <v>16</v>
       </c>
@@ -1633,43 +1610,43 @@
       <c r="A10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="8">
+      <c r="G10" s="5"/>
+      <c r="H10" s="6">
         <v>0.16049382716049382</v>
       </c>
-      <c r="I10" s="8">
-        <v>3.0737050417428601E-2</v>
-      </c>
-      <c r="J10" s="8">
-        <v>2.6636751826875499E-2</v>
-      </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="8">
+      <c r="I10" s="7">
+        <v>57.566666666666698</v>
+      </c>
+      <c r="J10" s="7">
+        <v>21.5</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="7">
+        <v>3500.2855321861098</v>
+      </c>
+      <c r="M10" s="7">
+        <v>705</v>
+      </c>
+      <c r="N10" s="6">
         <v>0.67433501078360891</v>
       </c>
-      <c r="O10" s="8">
-        <v>2.4649260912171501E-2</v>
-      </c>
-      <c r="P10" s="8">
-        <v>1.35331224724468E-3</v>
-      </c>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
       <c r="Q10" t="s">
         <v>36</v>
       </c>
@@ -1678,43 +1655,43 @@
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="8">
+      <c r="G11" s="5"/>
+      <c r="H11" s="6">
         <v>0.1419753086419753</v>
       </c>
-      <c r="I11" s="8">
-        <v>6.4594449344508295E-2</v>
-      </c>
-      <c r="J11" s="8">
-        <v>1.8285714285714301E-2</v>
-      </c>
-      <c r="K11" s="8">
+      <c r="I11" s="7">
+        <v>300.19230769230802</v>
+      </c>
+      <c r="J11" s="7">
+        <v>18</v>
+      </c>
+      <c r="K11" s="6">
         <v>0.3565934065934066</v>
       </c>
-      <c r="L11" s="8">
-        <v>6.6566917812788007E-2</v>
-      </c>
-      <c r="M11" s="8">
-        <v>2.5457438345266498E-2</v>
-      </c>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="7">
+        <v>1190.11620469083</v>
+      </c>
+      <c r="P11" s="7">
+        <v>44</v>
+      </c>
       <c r="Q11" t="s">
         <v>12</v>
       </c>
@@ -1723,49 +1700,45 @@
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="8">
+      <c r="G12" s="5"/>
+      <c r="H12" s="6">
         <v>0.22222222222222221</v>
       </c>
-      <c r="I12" s="8">
-        <v>8.82070812200728E-2</v>
-      </c>
-      <c r="J12" s="8">
-        <v>5.1828614328614298E-2</v>
-      </c>
-      <c r="K12" s="8">
+      <c r="I12" s="7">
+        <v>99.2173913043478</v>
+      </c>
+      <c r="J12" s="7">
+        <v>11</v>
+      </c>
+      <c r="K12" s="6">
         <v>0.61923076923076925</v>
       </c>
-      <c r="L12" s="8">
-        <v>6.2557279555679204E-2</v>
-      </c>
-      <c r="M12" s="8">
-        <v>2.40659710535173E-2</v>
-      </c>
-      <c r="N12" s="8">
+      <c r="L12" s="7">
+        <v>4827.8628659476099</v>
+      </c>
+      <c r="M12" s="7">
+        <v>925</v>
+      </c>
+      <c r="N12" s="6">
         <v>0.82458662832494611</v>
       </c>
-      <c r="O12" s="8">
-        <v>1.7651848753561499E-2</v>
-      </c>
-      <c r="P12" s="8">
-        <v>3.0030030030029999E-3</v>
-      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
       <c r="Q12" t="s">
         <v>22</v>
       </c>
@@ -1774,43 +1747,47 @@
       <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="8">
+      <c r="G13" s="5"/>
+      <c r="H13" s="6">
         <v>0.5</v>
       </c>
-      <c r="I13" s="8">
-        <v>0.13693990384485399</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="K13" s="8">
+      <c r="I13" s="7">
+        <v>290.83333333333297</v>
+      </c>
+      <c r="J13" s="7">
+        <v>35</v>
+      </c>
+      <c r="K13" s="6">
         <v>0.97692307692307689</v>
       </c>
-      <c r="L13" s="8">
-        <v>0.37180868483757401</v>
-      </c>
-      <c r="M13" s="8">
-        <v>0.318374772067609</v>
-      </c>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
+      <c r="L13" s="7">
+        <v>4076.8163265306098</v>
+      </c>
+      <c r="M13" s="7">
+        <v>708</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="7">
+        <v>972.36268526591095</v>
+      </c>
+      <c r="P13" s="7">
+        <v>105</v>
+      </c>
       <c r="Q13" t="s">
         <v>32</v>
       </c>
@@ -1819,37 +1796,37 @@
       <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="8">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6">
         <v>0.36419753086419754</v>
       </c>
-      <c r="I14" s="8">
-        <v>8.0500854033508998E-2</v>
-      </c>
-      <c r="J14" s="8">
-        <v>4.0358744394618798E-2</v>
-      </c>
-      <c r="K14" s="8">
+      <c r="I14" s="7">
+        <v>181.07407407407399</v>
+      </c>
+      <c r="J14" s="7">
+        <v>14</v>
+      </c>
+      <c r="K14" s="6">
         <v>0.85274725274725272</v>
       </c>
-      <c r="L14" s="8">
-        <v>7.8179753431432297E-2</v>
-      </c>
-      <c r="M14" s="8">
-        <v>2.26516193470216E-2</v>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
+      <c r="L14" s="7">
+        <v>25634.120359954999</v>
+      </c>
+      <c r="M14" s="7">
+        <v>9993.5</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
       <c r="Q14" t="s">
         <v>30</v>
       </c>
@@ -1858,50 +1835,50 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="6">
         <v>0.10493827160493827</v>
       </c>
-      <c r="I15" s="8">
-        <v>4.2517926762829797E-2</v>
-      </c>
-      <c r="J15" s="8">
-        <v>1.6853932584269701E-2</v>
-      </c>
-      <c r="K15" s="8">
+      <c r="I15" s="7">
+        <v>67</v>
+      </c>
+      <c r="J15" s="7">
+        <v>7</v>
+      </c>
+      <c r="K15" s="6">
         <v>0.68131868131868134</v>
       </c>
-      <c r="L15" s="8">
-        <v>2.37142588305366E-2</v>
-      </c>
-      <c r="M15" s="8">
-        <v>6.1717192086218099E-3</v>
-      </c>
-      <c r="N15" s="8">
+      <c r="L15" s="7">
+        <v>1589.1298387096799</v>
+      </c>
+      <c r="M15" s="7">
+        <v>182.5</v>
+      </c>
+      <c r="N15" s="6">
         <v>0.56578001437814518</v>
       </c>
-      <c r="O15" s="8">
-        <v>1.21891501817768E-2</v>
-      </c>
-      <c r="P15" s="8">
-        <v>1.4695077149155E-3</v>
+      <c r="O15" s="7">
+        <v>755.93138500635303</v>
+      </c>
+      <c r="P15" s="7">
+        <v>51</v>
       </c>
       <c r="Q15" t="s">
         <v>8</v>
@@ -1911,46 +1888,46 @@
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="8">
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6">
         <v>0.19753086419753085</v>
       </c>
-      <c r="I16" s="8">
-        <v>0.123766179546073</v>
-      </c>
-      <c r="J16" s="8">
-        <v>2.32837208023427E-2</v>
-      </c>
-      <c r="K16" s="8">
+      <c r="I16" s="7">
+        <v>38.5625</v>
+      </c>
+      <c r="J16" s="7">
+        <v>10</v>
+      </c>
+      <c r="K16" s="6">
         <v>0.61538461538461542</v>
       </c>
-      <c r="L16" s="8">
-        <v>1.20569127735507E-2</v>
-      </c>
-      <c r="M16" s="8">
-        <v>1.5507838784936401E-3</v>
-      </c>
-      <c r="N16" s="8">
+      <c r="L16" s="7">
+        <v>494.94464285714298</v>
+      </c>
+      <c r="M16" s="7">
+        <v>31</v>
+      </c>
+      <c r="N16" s="6">
         <v>0.68439971243709563</v>
       </c>
-      <c r="O16" s="8">
-        <v>0.15658377539139801</v>
-      </c>
-      <c r="P16" s="8">
-        <v>2.9048021441245998E-2</v>
+      <c r="O16" s="7">
+        <v>9887.9747899159702</v>
+      </c>
+      <c r="P16" s="7">
+        <v>712.5</v>
       </c>
       <c r="Q16" t="s">
         <v>18</v>
@@ -1960,46 +1937,46 @@
       <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="8">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6">
         <v>0.31481481481481483</v>
       </c>
-      <c r="I17" s="8">
-        <v>0.14328800462893501</v>
-      </c>
-      <c r="J17" s="8">
-        <v>4.15512465373961E-2</v>
-      </c>
-      <c r="K17" s="8">
+      <c r="I17" s="7">
+        <v>176.49019607843101</v>
+      </c>
+      <c r="J17" s="7">
+        <v>32</v>
+      </c>
+      <c r="K17" s="6">
         <v>0.34890109890109888</v>
       </c>
-      <c r="L17" s="8">
-        <v>1.16899128776664E-2</v>
-      </c>
-      <c r="M17" s="8">
-        <v>1.1591435974362501E-3</v>
-      </c>
-      <c r="N17" s="8">
+      <c r="L17" s="7">
+        <v>308.16692913385799</v>
+      </c>
+      <c r="M17" s="7">
+        <v>31</v>
+      </c>
+      <c r="N17" s="6">
         <v>0.7541337167505392</v>
       </c>
-      <c r="O17" s="8">
-        <v>0.16184178499517199</v>
-      </c>
-      <c r="P17" s="8">
-        <v>5.8574734658048001E-2</v>
+      <c r="O17" s="7">
+        <v>10210.429933269799</v>
+      </c>
+      <c r="P17" s="7">
+        <v>1372</v>
       </c>
       <c r="Q17" t="s">
         <v>28</v>
@@ -2009,50 +1986,50 @@
       <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="6">
         <v>0.18518518518518517</v>
       </c>
-      <c r="I18" s="8">
-        <v>2.52113768968589E-2</v>
-      </c>
-      <c r="J18" s="8">
-        <v>1.12033871216241E-2</v>
-      </c>
-      <c r="K18" s="8">
+      <c r="I18" s="7">
+        <v>70.566666666666706</v>
+      </c>
+      <c r="J18" s="7">
+        <v>43.5</v>
+      </c>
+      <c r="K18" s="6">
         <v>0.74890109890109891</v>
       </c>
-      <c r="L18" s="8">
-        <v>2.28801565521029E-2</v>
-      </c>
-      <c r="M18" s="8">
-        <v>4.1627950195130999E-3</v>
-      </c>
-      <c r="N18" s="8">
+      <c r="L18" s="7">
+        <v>1568.6471019809201</v>
+      </c>
+      <c r="M18" s="7">
+        <v>97</v>
+      </c>
+      <c r="N18" s="6">
         <v>0.61250898634076201</v>
       </c>
-      <c r="O18" s="8">
-        <v>1.5533504127972299E-2</v>
-      </c>
-      <c r="P18" s="8">
-        <v>1.6469986325979499E-3</v>
+      <c r="O18" s="7">
+        <v>939.58920187793399</v>
+      </c>
+      <c r="P18" s="7">
+        <v>46</v>
       </c>
       <c r="Q18" t="s">
         <v>14</v>
@@ -2062,45 +2039,45 @@
       <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="6">
         <v>0.25308641975308643</v>
       </c>
-      <c r="I19" s="8">
-        <v>0.45501447646592302</v>
-      </c>
-      <c r="J19" s="8">
-        <v>0.45045045045045001</v>
-      </c>
-      <c r="K19" s="8">
+      <c r="I19" s="7">
+        <v>245.707317073171</v>
+      </c>
+      <c r="J19" s="7">
+        <v>121</v>
+      </c>
+      <c r="K19" s="6">
         <v>0.34780219780219779</v>
       </c>
-      <c r="L19" s="8">
-        <v>6.7104408113115396E-2</v>
-      </c>
-      <c r="M19" s="8">
-        <v>1.1599290119522701E-2</v>
-      </c>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
+      <c r="L19" s="7">
+        <v>1167.48815165877</v>
+      </c>
+      <c r="M19" s="7">
+        <v>378</v>
+      </c>
+      <c r="N19" s="6"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
       <c r="Q19" t="s">
         <v>24</v>
       </c>

</xml_diff>